<commit_message>
Bugfixes and printing options
</commit_message>
<xml_diff>
--- a/test_files/hydroformylation.xlsx
+++ b/test_files/hydroformylation.xlsx
@@ -25,34 +25,34 @@
     <t xml:space="preserve">Catalyst</t>
   </si>
   <si>
-    <t xml:space="preserve">Structure 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS3,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS5,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure 6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS6,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure 7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TS7,2</t>
+    <t xml:space="preserve">ΔGRRS(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(TS1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(TS2) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(TS3)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ΔGRRS(TS4)  </t>
   </si>
   <si>
     <t xml:space="preserve">Product</t>
@@ -156,7 +156,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -177,12 +177,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Cantarell"/>
-      <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -258,7 +252,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -270,15 +264,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -302,43 +296,43 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="B2:L31"/>
+      <selection pane="topLeft" activeCell="P16" activeCellId="0" sqref="P16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="987" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">

</xml_diff>